<commit_message>
ADM1p compatible with modified ASM2d
</commit_message>
<xml_diff>
--- a/qsdsan/data/_masm2d.xlsx
+++ b/qsdsan/data/_masm2d.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\QSDsan\qsdsan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F49E428-BB99-46EF-9412-F526DC0B1D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BDBBFA-0A3D-45CA-9785-345DAA0D9116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="2235" windowWidth="20730" windowHeight="12315" activeTab="3" xr2:uid="{028F6E0F-965C-4F8B-87F9-99B413BFCEEA}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{028F6E0F-965C-4F8B-87F9-99B413BFCEEA}"/>
   </bookViews>
   <sheets>
     <sheet name="mASM2d" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="782">
   <si>
     <t>S_I</t>
   </si>
@@ -3318,38 +3318,38 @@
     <t>Ksp (mass based, e.g., mg/L) - GPS-X</t>
   </si>
   <si>
+    <t>k*[X_MeOH][S_PO4]* [X_MeOH]/([X_MeOH]]+K_X_MeOH)</t>
+  </si>
+  <si>
+    <t>mass-based stoichiometry</t>
+  </si>
+  <si>
+    <t>Precipitation/dissolution rate (mg/L precipitate /d); precipitate mass include the H2O in crystal</t>
+  </si>
+  <si>
+    <t>CaCO3_precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>struvite_precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>newberyite_precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>ACP _precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>MgCO3_precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>AlPO4_precipitation_dissolution</t>
+  </si>
+  <si>
+    <t>FePO4_precipitation_dissolution</t>
+  </si>
+  <si>
     <t>k*([A]^a*[B]^b - Ksp)* [X_AB]/([X_AB]+K_AB)          if [X_AB] &gt; 0
-k*([A]^a*[B]^b)                                                                 if [X_AB] = 0</t>
-  </si>
-  <si>
-    <t>k*[X_MeOH][S_PO4]* [X_MeOH]/([X_MeOH]]+K_X_MeOH)</t>
-  </si>
-  <si>
-    <t>mass-based stoichiometry</t>
-  </si>
-  <si>
-    <t>Precipitation/dissolution rate (mg/L precipitate /d); precipitate mass include the H2O in crystal</t>
-  </si>
-  <si>
-    <t>CaCO3_precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>struvite_precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>newberyite_precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>ACP _precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>MgCO3_precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>AlPO4_precipitation_dissolution</t>
-  </si>
-  <si>
-    <t>FePO4_precipitation_dissolution</t>
+k*([A]^a*[B]^b)                                                                          if [X_AB] = 0</t>
   </si>
 </sst>
 </file>
@@ -3875,25 +3875,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0B15A-AC83-4EBC-A6B6-CED6023B9B26}">
-  <dimension ref="A1:AI29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23:B29"/>
+      <selection pane="bottomRight" activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="30" width="9.140625" style="1"/>
-    <col min="31" max="32" width="9.140625" style="2"/>
-    <col min="33" max="33" width="61.7109375" style="4" customWidth="1"/>
-    <col min="34" max="35" width="79.28515625" style="4" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="2"/>
+    <col min="23" max="23" width="61.7109375" style="4" customWidth="1"/>
+    <col min="24" max="25" width="79.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>4</v>
       </c>
@@ -3948,50 +3947,20 @@
       <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="AE1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4016,17 +3985,17 @@
       <c r="O2">
         <v>-1</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4051,17 +4020,17 @@
       <c r="O3">
         <v>-1</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AH3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4086,17 +4055,17 @@
       <c r="O4">
         <v>-1</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4121,17 +4090,17 @@
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4156,17 +4125,17 @@
       <c r="P6">
         <v>1</v>
       </c>
-      <c r="AG6" s="4" t="s">
+      <c r="W6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AH6" s="4" t="s">
+      <c r="X6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="Y6" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4194,17 +4163,17 @@
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="AG7" s="4" t="s">
+      <c r="W7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AH7" s="4" t="s">
+      <c r="X7" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AI7" s="4" t="s">
+      <c r="Y7" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4232,17 +4201,17 @@
       <c r="P8">
         <v>1</v>
       </c>
-      <c r="AG8" s="4" t="s">
+      <c r="W8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AH8" s="4" t="s">
+      <c r="X8" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AI8" s="4" t="s">
+      <c r="Y8" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4264,17 +4233,17 @@
       <c r="K9" t="s">
         <v>20</v>
       </c>
-      <c r="AG9" s="4" t="s">
+      <c r="W9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AH9" s="4" t="s">
+      <c r="X9" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="AI9" s="4" t="s">
+      <c r="Y9" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4299,17 +4268,17 @@
       <c r="P10">
         <v>-1</v>
       </c>
-      <c r="AG10" s="4" t="s">
+      <c r="W10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AH10" s="4" t="s">
+      <c r="X10" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="AI10" s="4" t="s">
+      <c r="Y10" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4350,17 +4319,17 @@
         <v>1</v>
       </c>
       <c r="T11" s="7"/>
-      <c r="AG11" s="5" t="s">
+      <c r="W11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AH11" s="5" t="s">
+      <c r="X11" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="AI11" s="5" t="s">
+      <c r="Y11" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4401,17 +4370,17 @@
         <v>48</v>
       </c>
       <c r="T12" s="7"/>
-      <c r="AG12" s="5" t="s">
+      <c r="W12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AH12" s="5" t="s">
+      <c r="X12" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="AI12" s="5" t="s">
+      <c r="Y12" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -4454,17 +4423,17 @@
         <v>48</v>
       </c>
       <c r="T13" s="7"/>
-      <c r="AG13" s="5" t="s">
+      <c r="W13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AH13" s="5" t="s">
+      <c r="X13" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="AI13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4494,17 +4463,17 @@
         <v>51</v>
       </c>
       <c r="T14" s="7"/>
-      <c r="AG14" s="5" t="s">
+      <c r="W14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AH14" s="4" t="s">
+      <c r="X14" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="AI14" s="4" t="s">
+      <c r="Y14" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -4537,17 +4506,17 @@
         <v>51</v>
       </c>
       <c r="T15" s="7"/>
-      <c r="AG15" s="5" t="s">
+      <c r="W15" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AH15" s="4" t="s">
+      <c r="X15" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="AI15" s="4" t="s">
+      <c r="Y15" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4576,17 +4545,17 @@
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
-      <c r="AG16" s="5" t="s">
+      <c r="W16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AH16" s="4" t="s">
+      <c r="X16" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="AI16" s="4" t="s">
+      <c r="Y16" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4623,17 +4592,17 @@
       </c>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="AG17" s="5" t="s">
+      <c r="W17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AH17" s="5" t="s">
+      <c r="X17" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="AI17" s="5" t="s">
+      <c r="Y17" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4652,17 +4621,17 @@
       <c r="S18">
         <v>-1</v>
       </c>
-      <c r="AG18" s="5" t="s">
+      <c r="W18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AH18" s="4" t="s">
+      <c r="X18" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="AI18" s="4" t="s">
+      <c r="Y18" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4687,17 +4656,17 @@
       <c r="T19">
         <v>1</v>
       </c>
-      <c r="AG19" s="4" t="s">
+      <c r="W19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AH19" s="4" t="s">
+      <c r="X19" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="AI19" s="4" t="s">
+      <c r="Y19" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4722,17 +4691,17 @@
       <c r="T20">
         <v>-1</v>
       </c>
-      <c r="AG20" s="4" t="s">
+      <c r="W20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AH20" s="4" t="s">
+      <c r="X20" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="AI20" s="4" t="s">
+      <c r="Y20" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>69</v>
       </c>
@@ -4742,29 +4711,19 @@
       <c r="K21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="2">
+      <c r="U21" s="2">
         <v>-3.45</v>
       </c>
-      <c r="AF21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG21" s="6" t="s">
+      <c r="V21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-    </row>
-    <row r="22" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>71</v>
       </c>
@@ -4774,58 +4733,38 @@
       <c r="K22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y22"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-      <c r="AC22"/>
-      <c r="AD22"/>
-      <c r="AE22" s="2">
+      <c r="U22" s="2">
         <v>3.45</v>
       </c>
-      <c r="AF22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG22" s="6" t="s">
+      <c r="V22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>781</v>
-      </c>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12562,8 +12501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4592AAF9-B2E1-421A-B561-417BA0A852F0}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13184,7 +13123,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -13193,7 +13132,7 @@
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13229,7 +13168,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>771</v>
+        <v>781</v>
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
@@ -13327,7 +13266,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="13">
-        <f t="shared" ref="C33:H33" si="8">C8*C$13/$L13</f>
+        <f t="shared" ref="C33:G33" si="8">C8*C$13/$L13</f>
         <v>-0.38762653942871883</v>
       </c>
       <c r="D33" s="13">
@@ -13431,7 +13370,7 @@
         <v>-0.25398738007380073</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -13579,7 +13518,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -13593,7 +13532,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -13610,7 +13549,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -13624,7 +13563,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C5">
         <v>-3</v>
@@ -13638,7 +13577,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -13652,7 +13591,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -13666,7 +13605,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E8">
         <v>-1</v>

</xml_diff>